<commit_message>
PF-2721: update excel templates to include "Proposal" as a Project Stage option. Update menu item, page title, and instructions to include "Proposal"
</commit_message>
<xml_diff>
--- a/Source/ProjectFirma.Web/Content/excel-templates/ClackamasPartnership/Pending Projects Template.xlsx
+++ b/Source/ProjectFirma.Web/Content/excel-templates/ClackamasPartnership/Pending Projects Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\projectfirma\Source\ProjectFirma.Web\Content\excel-templates\ClackamasPartnership\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2972E932-85EA-4631-AEB5-CADD6E11C823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71167246-B432-4E06-9AAC-84C7E072196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9405" yWindow="8250" windowWidth="45300" windowHeight="23430" tabRatio="820" xr2:uid="{78B30058-8F2E-4265-9AEE-7F618CBAC47F}"/>
+    <workbookView xWindow="21825" yWindow="5895" windowWidth="35040" windowHeight="24105" tabRatio="820" xr2:uid="{78B30058-8F2E-4265-9AEE-7F618CBAC47F}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="19" r:id="rId1"/>
@@ -168,9 +168,34 @@
     <t>Required if Project Stage is Completed</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
+    <t>ESA Sitka</t>
+  </si>
+  <si>
+    <t>Simple Location Notes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">INSTRUCTIONS
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;Enter data for a Project in the Basics tab of the template. Required attributes are listed below.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required if Lat/Long are blank
+</t>
+    </r>
+    <r>
+      <rPr>
         <i/>
         <sz val="10"/>
         <color theme="1"/>
@@ -178,68 +203,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Required
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Options are:
-Deferred, Planning/Design, Terminated, 
-Implementation, Post-Implementation,
-Completed</t>
-    </r>
-  </si>
-  <si>
-    <t>ESA Sitka</t>
-  </si>
-  <si>
-    <t>Pending Project Reporting Template</t>
-  </si>
-  <si>
-    <t>Simple Location Notes</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">INSTRUCTIONS
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&gt;Enter data for a Project in the Basics tab of the template. Required attributes are listed below.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Required if Lat/Long are blank
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>4000 character limit</t>
     </r>
-  </si>
-  <si>
-    <t>Use this template to upload new pending projects to the Clackamas Partnership Project Tracker in bulk.</t>
   </si>
   <si>
     <r>
@@ -347,6 +312,41 @@
   </si>
   <si>
     <t>Upslope Land Uses</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Required
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Options are:
+Proposal, Deferred, Planning/Design,
+Terminated, Implementation,
+Post-Implementation, Completed</t>
+    </r>
+  </si>
+  <si>
+    <t>Proposal and Pending Project Reporting Template</t>
+  </si>
+  <si>
+    <t>Use this template to upload new proposals and pending projects to the Clackamas Partnership Project Tracker in bulk.</t>
   </si>
 </sst>
 </file>
@@ -870,23 +870,23 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="255" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -942,7 +942,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -970,7 +970,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>18</v>
@@ -991,13 +991,13 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="12" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
@@ -1008,10 +1008,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -1029,13 +1029,13 @@
         <v>15</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>5</v>
@@ -1068,7 +1068,7 @@
         <v>16</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>10</v>
@@ -1090,7 +1090,7 @@
       <formula1>500</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576" xr:uid="{1A7D9C65-0473-493F-A453-B95D7AA5CA7E}">
-      <formula1>"Deffered, Planning/Design, Terminated, Implementation, Post-Implementation, Completed"</formula1>
+      <formula1>"Proposal, Deffered, Planning/Design, Terminated, Implementation, Post-Implementation, Completed"</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds Character Limit" error="Description can have no more than 4000 characters" sqref="B4:B1048576" xr:uid="{CD7E6673-0D1D-4C81-AAE8-176F3732CD4A}">
       <formula1>4000</formula1>
@@ -1147,7 +1147,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>